<commit_message>
BOM updated with 2.1 schematic
</commit_message>
<xml_diff>
--- a/2. Mounting/Bill of Materials.xlsx
+++ b/2. Mounting/Bill of Materials.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Senaino\Senaino\2. Mounting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiago Silva\Desktop\New folder (3)\Senaino\2. Mounting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30EF0A4A-5C53-4787-A128-C2FF9CF1590A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8C9EC8D-BCE1-45C9-AAD1-9EFF36112842}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10920" yWindow="1770" windowWidth="28800" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19200" yWindow="3810" windowWidth="19200" windowHeight="10665" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MONTAGEM" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="64">
   <si>
     <t>C1</t>
   </si>
@@ -1157,8 +1157,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1340,7 +1340,7 @@
         <v>17</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -1348,7 +1348,7 @@
         <v>18</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>